<commit_message>
Adjust Mutation Probs by what events frequency
</commit_message>
<xml_diff>
--- a/PythonEnvironment/resources/all_results.xlsx
+++ b/PythonEnvironment/resources/all_results.xlsx
@@ -3169,11 +3169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1592139728"/>
-        <c:axId val="-1592137952"/>
+        <c:axId val="-1114010016"/>
+        <c:axId val="-1145199632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1592139728"/>
+        <c:axId val="-1114010016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -3286,12 +3286,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1592137952"/>
+        <c:crossAx val="-1145199632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1592137952"/>
+        <c:axId val="-1145199632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1592139728"/>
+        <c:crossAx val="-1114010016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,7 +4341,7 @@
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Use High Mutation Prob
</commit_message>
<xml_diff>
--- a/PythonEnvironment/resources/all_results.xlsx
+++ b/PythonEnvironment/resources/all_results.xlsx
@@ -553,154 +553,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.401515151515151</c:v>
+                  <c:v>0.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.348484848484848</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.477272727272727</c:v>
+                  <c:v>0.533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.401515151515151</c:v>
+                  <c:v>0.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.522727272727272</c:v>
+                  <c:v>0.516666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.568181818181818</c:v>
+                  <c:v>0.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.522727272727272</c:v>
+                  <c:v>0.516666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.454545454545454</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.431818181818181</c:v>
+                  <c:v>0.683333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.462121212121212</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.575757575757575</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.674242424242424</c:v>
+                  <c:v>0.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.719696969696969</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.772727272727272</c:v>
+                  <c:v>0.716666666666666</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.613636363636363</c:v>
+                  <c:v>0.683333333333333</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.674242424242424</c:v>
+                  <c:v>0.816666666666666</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.674242424242424</c:v>
+                  <c:v>0.816666666666666</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.636363636363636</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.636363636363636</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.651515151515151</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.545454545454545</c:v>
+                  <c:v>0.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.727272727272727</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.795454545454545</c:v>
+                  <c:v>0.816666666666666</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.681818181818181</c:v>
+                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.742424242424242</c:v>
+                  <c:v>0.783333333333333</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.712121212121212</c:v>
+                  <c:v>0.733333333333333</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.636363636363636</c:v>
+                  <c:v>0.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.674242424242424</c:v>
+                  <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.696969696969696</c:v>
+                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.537878787878787</c:v>
+                  <c:v>0.466666666666666</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.522727272727272</c:v>
+                  <c:v>0.433333333333333</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.484848484848484</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.575757575757575</c:v>
+                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.613636363636363</c:v>
+                  <c:v>0.633333333333333</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.53030303030303</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.568181818181818</c:v>
+                  <c:v>0.866666666666666</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.613636363636363</c:v>
+                  <c:v>0.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.515151515151515</c:v>
+                  <c:v>0.716666666666666</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.643939393939393</c:v>
+                  <c:v>0.649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.545454545454545</c:v>
+                  <c:v>0.683333333333333</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.575757575757575</c:v>
+                  <c:v>0.683333333333333</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.484848484848484</c:v>
+                  <c:v>0.783333333333333</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.613636363636363</c:v>
+                  <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.56060606060606</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.681818181818181</c:v>
+                  <c:v>0.783333333333333</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.765151515151515</c:v>
+                  <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.696969696969697</c:v>
+                  <c:v>0.749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.636363636363636</c:v>
+                  <c:v>0.783333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3169,11 +3169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1114010016"/>
-        <c:axId val="-1145199632"/>
+        <c:axId val="1603313392"/>
+        <c:axId val="1603354208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1114010016"/>
+        <c:axId val="1603313392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -3286,12 +3286,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1145199632"/>
+        <c:crossAx val="1603354208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1145199632"/>
+        <c:axId val="1603354208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1114010016"/>
+        <c:crossAx val="1603313392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,7 +4341,7 @@
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.40151515151515099</v>
+        <v>0.483333333333333</v>
       </c>
       <c r="D2">
         <v>0.3</v>
@@ -4388,7 +4388,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.34848484848484801</v>
+        <v>0.45</v>
       </c>
       <c r="D3">
         <v>0.55454545454545401</v>
@@ -4399,7 +4399,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.47727272727272702</v>
+        <v>0.53333333333333299</v>
       </c>
       <c r="D4">
         <v>0.53181818181818097</v>
@@ -4410,7 +4410,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.40151515151515099</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="D5">
         <v>0.67272727272727195</v>
@@ -4421,7 +4421,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.52272727272727204</v>
+        <v>0.51666666666666605</v>
       </c>
       <c r="D6">
         <v>0.62727272727272698</v>
@@ -4432,7 +4432,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.56818181818181801</v>
+        <v>0.483333333333333</v>
       </c>
       <c r="D7">
         <v>0.64545454545454495</v>
@@ -4443,7 +4443,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.52272727272727204</v>
+        <v>0.51666666666666605</v>
       </c>
       <c r="D8">
         <v>0.77272727272727204</v>
@@ -4454,7 +4454,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.45454545454545398</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
         <v>0.83636363636363598</v>
@@ -4465,7 +4465,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.43181818181818099</v>
+        <v>0.68333333333333302</v>
       </c>
       <c r="D10">
         <v>0.86363636363636298</v>
@@ -4476,7 +4476,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.46212121212121199</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
         <v>0.88636363636363602</v>
@@ -4487,7 +4487,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.57575757575757502</v>
+        <v>0.45</v>
       </c>
       <c r="D12">
         <v>0.86363636363636298</v>
@@ -4498,7 +4498,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.67424242424242398</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="D13">
         <v>0.79545454545454497</v>
@@ -4509,7 +4509,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.71969696969696895</v>
+        <v>0.75</v>
       </c>
       <c r="D14">
         <v>0.80909090909090897</v>
@@ -4520,7 +4520,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.77272727272727204</v>
+        <v>0.71666666666666601</v>
       </c>
       <c r="D15">
         <v>0.83181818181818101</v>
@@ -4531,7 +4531,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.83333333333333304</v>
+        <v>0.6</v>
       </c>
       <c r="D16">
         <v>0.88636363636363602</v>
@@ -4542,7 +4542,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.61363636363636298</v>
+        <v>0.68333333333333302</v>
       </c>
       <c r="D17">
         <v>0.88636363636363602</v>
@@ -4553,7 +4553,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.67424242424242398</v>
+        <v>0.81666666666666599</v>
       </c>
       <c r="D18">
         <v>0.90909090909090895</v>
@@ -4564,7 +4564,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="D19">
         <v>0.90909090909090895</v>
@@ -4575,7 +4575,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.67424242424242398</v>
+        <v>0.81666666666666599</v>
       </c>
       <c r="D20">
         <v>0.88636363636363602</v>
@@ -4586,7 +4586,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.63636363636363602</v>
+        <v>0.85</v>
       </c>
       <c r="D21">
         <v>0.82727272727272705</v>
@@ -4597,7 +4597,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.63636363636363602</v>
+        <v>0.8</v>
       </c>
       <c r="D22">
         <v>0.76818181818181797</v>
@@ -4608,7 +4608,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.65151515151515105</v>
+        <v>0.65</v>
       </c>
       <c r="D23">
         <v>0.88636363636363602</v>
@@ -4619,7 +4619,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.54545454545454497</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="D24">
         <v>0.79545454545454497</v>
@@ -4630,7 +4630,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.72727272727272696</v>
+        <v>0.91666666666666596</v>
       </c>
       <c r="D25">
         <v>0.90909090909090895</v>
@@ -4641,7 +4641,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.79545454545454497</v>
+        <v>0.81666666666666599</v>
       </c>
       <c r="D26">
         <v>0.85</v>
@@ -4652,7 +4652,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.68181818181818099</v>
+        <v>0.56666666666666599</v>
       </c>
       <c r="D27">
         <v>0.87272727272727202</v>
@@ -4663,7 +4663,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.74242424242424199</v>
+        <v>0.78333333333333299</v>
       </c>
       <c r="D28">
         <v>0.82727272727272705</v>
@@ -4674,7 +4674,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.71212121212121204</v>
+        <v>0.73333333333333295</v>
       </c>
       <c r="D29">
         <v>0.88636363636363602</v>
@@ -4685,7 +4685,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.63636363636363602</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D30">
         <v>0.75</v>
@@ -4696,7 +4696,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.67424242424242398</v>
+        <v>0.76666666666666605</v>
       </c>
       <c r="D31">
         <v>0.777272727272727</v>
@@ -4707,7 +4707,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.69696969696969602</v>
+        <v>0.56666666666666599</v>
       </c>
       <c r="D32">
         <v>0.75454545454545396</v>
@@ -4718,7 +4718,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.53787878787878696</v>
+        <v>0.46666666666666601</v>
       </c>
       <c r="D33">
         <v>0.77272727272727204</v>
@@ -4729,7 +4729,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.52272727272727204</v>
+        <v>0.43333333333333302</v>
       </c>
       <c r="D34">
         <v>0.77272727272727204</v>
@@ -4740,7 +4740,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.48484848484848397</v>
+        <v>0.4</v>
       </c>
       <c r="D35">
         <v>0.81818181818181801</v>
@@ -4751,7 +4751,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.57575757575757502</v>
+        <v>0.56666666666666599</v>
       </c>
       <c r="D36">
         <v>0.78636363636363604</v>
@@ -4762,7 +4762,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.61363636363636298</v>
+        <v>0.63333333333333297</v>
       </c>
       <c r="D37">
         <v>0.80454545454545401</v>
@@ -4773,7 +4773,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.53030303030303005</v>
+        <v>0.65</v>
       </c>
       <c r="D38">
         <v>0.777272727272727</v>
@@ -4784,7 +4784,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.56818181818181801</v>
+        <v>0.86666666666666603</v>
       </c>
       <c r="D39">
         <v>0.81363636363636305</v>
@@ -4795,7 +4795,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.61363636363636298</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="D40">
         <v>0.75909090909090904</v>
@@ -4806,7 +4806,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.51515151515151503</v>
+        <v>0.71666666666666601</v>
       </c>
       <c r="D41">
         <v>0.80909090909090897</v>
@@ -4817,7 +4817,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.64393939393939303</v>
+        <v>0.64999999999999902</v>
       </c>
       <c r="D42">
         <v>0.85909090909090902</v>
@@ -4828,7 +4828,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.54545454545454497</v>
+        <v>0.68333333333333302</v>
       </c>
       <c r="D43">
         <v>0.85909090909090902</v>
@@ -4839,7 +4839,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.57575757575757502</v>
+        <v>0.68333333333333302</v>
       </c>
       <c r="D44">
         <v>0.88636363636363602</v>
@@ -4850,7 +4850,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.48484848484848397</v>
+        <v>0.78333333333333299</v>
       </c>
       <c r="D45">
         <v>0.85909090909090902</v>
@@ -4861,7 +4861,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.61363636363636298</v>
+        <v>0.76666666666666605</v>
       </c>
       <c r="D46">
         <v>0.86363636363636298</v>
@@ -4872,7 +4872,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.56060606060606</v>
+        <v>0.91666666666666596</v>
       </c>
       <c r="D47">
         <v>0.76818181818181797</v>
@@ -4883,7 +4883,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.68181818181818099</v>
+        <v>0.78333333333333299</v>
       </c>
       <c r="D48">
         <v>0.85909090909090902</v>
@@ -4894,7 +4894,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.76515151515151503</v>
+        <v>0.76666666666666605</v>
       </c>
       <c r="D49">
         <v>0.88636363636363602</v>
@@ -4905,7 +4905,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.69696969696969702</v>
+        <v>0.749999999999999</v>
       </c>
       <c r="D50">
         <v>0.88636363636363602</v>
@@ -4916,7 +4916,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.63636363636363602</v>
+        <v>0.78333333333333299</v>
       </c>
       <c r="D51">
         <v>0.88636363636363602</v>

</xml_diff>

<commit_message>
Add Data to spreaddsheet
</commit_message>
<xml_diff>
--- a/PythonEnvironment/resources/all_results.xlsx
+++ b/PythonEnvironment/resources/all_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Gen</t>
   </si>
@@ -47,9 +47,6 @@
     <t>E,F,X,W</t>
   </si>
   <si>
-    <t>F,X,F,E,F,W</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -57,6 +54,12 @@
   </si>
   <si>
     <t>F,W</t>
+  </si>
+  <si>
+    <t>F,F,X,E,W</t>
+  </si>
+  <si>
+    <t>levels not very interesting</t>
   </si>
 </sst>
 </file>
@@ -238,313 +241,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -556,151 +411,154 @@
                   <c:v>0.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45</c:v>
+                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.666666666666666</c:v>
+                  <c:v>0.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.483333333333333</c:v>
+                  <c:v>0.466666666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.383333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.616666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.683333333333333</c:v>
+                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.45</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.666666666666666</c:v>
+                  <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.75</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.716666666666666</c:v>
+                  <c:v>0.649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.6</c:v>
+                  <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.683333333333333</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0.766666666666666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.866666666666666</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.866666666666666</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>0.816666666666666</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.816666666666666</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
+                  <c:v>0.866666666666666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.916666666666666</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.816666666666666</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.566666666666666</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.783333333333333</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>0.766666666666666</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.883333333333333</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.866666666666666</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.883333333333333</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.783333333333333</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.816666666666666</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0.733333333333333</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.583333333333333</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.766666666666666</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.466666666666666</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.433333333333333</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.566666666666666</c:v>
-                </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.633333333333333</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.65</c:v>
+                  <c:v>0.733333333333333</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.866666666666666</c:v>
+                  <c:v>0.816666666666666</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.666666666666666</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.716666666666666</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.649999999999999</c:v>
+                  <c:v>0.916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.683333333333333</c:v>
+                  <c:v>0.966666666666666</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.683333333333333</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.783333333333333</c:v>
+                  <c:v>0.883333333333333</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0.766666666666666</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0.866666666666666</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>0.916666666666666</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.783333333333333</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.766666666666666</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.749999999999999</c:v>
+                  <c:v>0.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.783333333333333</c:v>
+                  <c:v>0.816666666666666</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,313 +604,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1060,6 +770,159 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.829999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.909999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.939999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.909999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.829999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1104,313 +967,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1567,156 +1282,6 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0.886363636363636</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.813636363636363</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.886363636363636</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.909090909090909</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.886363636363636</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.881818181818181</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.886363636363636</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.795454545454545</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.795454545454545</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.836363636363636</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.627272727272727</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.813636363636363</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.836363636363636</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.84090909090909</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.813636363636363</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.727272727272727</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.84090909090909</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.84090909090909</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.781818181818181</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.781818181818182</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.759090909090909</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.736363636363636</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.818181818181818</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.84090909090909</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.863636363636363</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.909090909090909</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.818181818181818</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.777272727272727</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.759090909090909</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.827272727272727</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.818181818181818</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.722727272727272</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.818181818181818</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.69090909090909</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.759090909090909</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.831818181818181</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.772727272727272</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.84090909090909</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.813636363636363</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.727272727272727</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.836363636363636</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.772727272727272</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.809090909090909</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.759090909090909</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.786363636363636</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.836363636363636</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.731818181818181</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.795454545454545</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1762,313 +1327,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2120,313 +1537,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2478,313 +1747,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2806,7 +1927,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>F,X,F,E,F,W</c:v>
+                  <c:v>F,F,X,E,W</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2842,313 +1963,165 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+              <c:strCache>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Notes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -3156,6 +2129,156 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.255555555555555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.322222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.388888888888888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.416666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.366666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.372222222222222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.277777777777777</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.161111111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.238888888888888</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.177777777777777</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.155555555555555</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.155555555555555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.316666666666666</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.238888888888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.272222222222222</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.244444444444444</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.244444444444444</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.366666666666666</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.316666666666666</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.516666666666666</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.355555555555555</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.216666666666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.0944444444444444</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.233333333333333</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.244444444444444</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.366666666666666</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.344444444444444</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.388888888888888</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.388888888888888</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.144444444444444</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.155555555555555</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.211111111111111</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.266666666666666</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.161111111111111</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.244444444444444</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.394444444444444</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.311111111111111</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.322222222222222</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.277777777777777</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3169,11 +2292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1603313392"/>
-        <c:axId val="1603354208"/>
+        <c:axId val="1641237712"/>
+        <c:axId val="1641239840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1603313392"/>
+        <c:axId val="1641237712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -3286,14 +2409,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1603354208"/>
+        <c:crossAx val="1641239840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1603354208"/>
+        <c:axId val="1641239840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3403,7 +2527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1603313392"/>
+        <c:crossAx val="1641237712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4338,10 +3462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C51"/>
+    <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4351,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4369,7 +3493,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4379,8 +3503,14 @@
       <c r="B2">
         <v>0.483333333333333</v>
       </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
       <c r="D2">
         <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>0.25555555555555498</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -4388,10 +3518,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.45</v>
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="C3">
+        <v>0.59</v>
       </c>
       <c r="D3">
         <v>0.55454545454545401</v>
+      </c>
+      <c r="H3">
+        <v>0.32222222222222202</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -4401,8 +3537,14 @@
       <c r="B4">
         <v>0.53333333333333299</v>
       </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
       <c r="D4">
         <v>0.53181818181818097</v>
+      </c>
+      <c r="H4">
+        <v>0.33333333333333298</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -4410,10 +3552,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.66666666666666596</v>
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="C5">
+        <v>0.76</v>
       </c>
       <c r="D5">
         <v>0.67272727272727195</v>
+      </c>
+      <c r="H5">
+        <v>0.38888888888888801</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -4421,10 +3569,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.51666666666666605</v>
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="C6">
+        <v>0.52</v>
       </c>
       <c r="D6">
         <v>0.62727272727272698</v>
+      </c>
+      <c r="H6">
+        <v>0.41666666666666602</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -4432,10 +3586,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.483333333333333</v>
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="C7">
+        <v>0.64</v>
       </c>
       <c r="D7">
         <v>0.64545454545454495</v>
+      </c>
+      <c r="H7">
+        <v>0.36666666666666597</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -4443,10 +3603,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.51666666666666605</v>
+        <v>0.38333333333333303</v>
+      </c>
+      <c r="C8">
+        <v>0.77</v>
       </c>
       <c r="D8">
         <v>0.77272727272727204</v>
+      </c>
+      <c r="H8">
+        <v>0.37222222222222201</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4454,10 +3620,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.61666666666666603</v>
+      </c>
+      <c r="C9">
+        <v>0.78</v>
       </c>
       <c r="D9">
         <v>0.83636363636363598</v>
+      </c>
+      <c r="H9">
+        <v>0.27777777777777701</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4465,10 +3637,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.68333333333333302</v>
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="C10">
+        <v>0.69</v>
       </c>
       <c r="D10">
         <v>0.86363636363636298</v>
+      </c>
+      <c r="H10">
+        <v>0.16111111111111101</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -4476,10 +3654,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C11">
+        <v>0.66</v>
       </c>
       <c r="D11">
         <v>0.88636363636363602</v>
+      </c>
+      <c r="H11">
+        <v>0.23888888888888801</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4487,10 +3671,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.45</v>
+        <v>0.65</v>
+      </c>
+      <c r="C12">
+        <v>0.749999999999999</v>
       </c>
       <c r="D12">
         <v>0.86363636363636298</v>
+      </c>
+      <c r="H12">
+        <v>0.33333333333333298</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -4498,10 +3688,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.66666666666666596</v>
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="C13">
+        <v>0.65</v>
       </c>
       <c r="D13">
         <v>0.79545454545454497</v>
+      </c>
+      <c r="H13">
+        <v>0.17777777777777701</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -4509,10 +3705,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.75</v>
+        <v>0.65</v>
+      </c>
+      <c r="C14">
+        <v>0.79</v>
       </c>
       <c r="D14">
         <v>0.80909090909090897</v>
+      </c>
+      <c r="H14">
+        <v>0.155555555555555</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -4520,10 +3722,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.71666666666666601</v>
+        <v>0.64999999999999902</v>
+      </c>
+      <c r="C15">
+        <v>0.73</v>
       </c>
       <c r="D15">
         <v>0.83181818181818101</v>
+      </c>
+      <c r="H15">
+        <v>0.155555555555555</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -4531,803 +3739,622 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.6</v>
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="C16">
+        <v>0.84</v>
       </c>
       <c r="D16">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.68333333333333302</v>
+        <v>0.9</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
       </c>
       <c r="D17">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>0.31666666666666599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.81666666666666599</v>
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="C18">
+        <v>0.77999999999999903</v>
       </c>
       <c r="D18">
         <v>0.90909090909090895</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>0.23888888888888801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.8</v>
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C19">
+        <v>0.85</v>
       </c>
       <c r="D19">
         <v>0.90909090909090895</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.81666666666666599</v>
+        <v>0.8</v>
+      </c>
+      <c r="C20">
+        <v>0.71</v>
       </c>
       <c r="D20">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>0.27222222222222198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.85</v>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="C21">
+        <v>0.8</v>
       </c>
       <c r="D21">
         <v>0.82727272727272705</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>0.24444444444444399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.8</v>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="C22">
+        <v>0.83</v>
       </c>
       <c r="D22">
         <v>0.76818181818181797</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.65</v>
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="C23">
+        <v>0.84</v>
       </c>
       <c r="D23">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>4.4444444444444398E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.66666666666666596</v>
+        <v>0.8</v>
+      </c>
+      <c r="C24">
+        <v>0.82999999999999896</v>
       </c>
       <c r="D24">
         <v>0.79545454545454497</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>0.22222222222222199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.91666666666666596</v>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="C25">
+        <v>0.8</v>
       </c>
       <c r="D25">
         <v>0.90909090909090895</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>0.24444444444444399</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.81666666666666599</v>
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C26">
+        <v>0.90999999999999903</v>
       </c>
       <c r="D26">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>0.36666666666666597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.56666666666666599</v>
+        <v>0.8</v>
+      </c>
+      <c r="C27">
+        <v>0.94</v>
       </c>
       <c r="D27">
         <v>0.87272727272727202</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <v>0.78333333333333299</v>
       </c>
+      <c r="C28">
+        <v>0.9</v>
+      </c>
       <c r="D28">
         <v>0.82727272727272705</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>0.31666666666666599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.73333333333333295</v>
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="C29">
+        <v>0.72</v>
       </c>
       <c r="D29">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>0.51666666666666605</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.58333333333333304</v>
+        <v>0.88333333333333297</v>
+      </c>
+      <c r="C30">
+        <v>0.85</v>
       </c>
       <c r="D30">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>0.35555555555555501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.76666666666666605</v>
+        <v>0.8</v>
+      </c>
+      <c r="C31">
+        <v>0.93999999999999895</v>
       </c>
       <c r="D31">
         <v>0.777272727272727</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>0.21666666666666601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.56666666666666599</v>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="C32">
+        <v>0.9</v>
       </c>
       <c r="D32">
         <v>0.75454545454545396</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>9.44444444444444E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.46666666666666601</v>
+        <v>0.88333333333333297</v>
+      </c>
+      <c r="C33">
+        <v>0.91</v>
       </c>
       <c r="D33">
         <v>0.77272727272727204</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>0.233333333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.43333333333333302</v>
+        <v>0.78333333333333299</v>
+      </c>
+      <c r="C34">
+        <v>0.74</v>
       </c>
       <c r="D34">
         <v>0.77272727272727204</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>0.19999999999999901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.4</v>
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="C35">
+        <v>0.75</v>
       </c>
       <c r="D35">
         <v>0.81818181818181801</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.56666666666666599</v>
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="C36">
+        <v>0.96</v>
       </c>
       <c r="D36">
         <v>0.78636363636363604</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>0.24444444444444399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.63333333333333297</v>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="C37">
+        <v>0.97</v>
       </c>
       <c r="D37">
         <v>0.80454545454545401</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>0.36666666666666597</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.65</v>
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="C38">
+        <v>0.97</v>
       </c>
       <c r="D38">
         <v>0.777272727272727</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>0.344444444444444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.86666666666666603</v>
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="C39">
+        <v>0.90999999999999903</v>
       </c>
       <c r="D39">
         <v>0.81363636363636305</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>0.38888888888888801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.66666666666666596</v>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="C40">
+        <v>0.79</v>
       </c>
       <c r="D40">
         <v>0.75909090909090904</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <v>0.38888888888888801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.71666666666666601</v>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="C41">
+        <v>0.84</v>
       </c>
       <c r="D41">
         <v>0.80909090909090897</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>0.14444444444444399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.64999999999999902</v>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="C42">
+        <v>0.82</v>
       </c>
       <c r="D42">
         <v>0.85909090909090902</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.68333333333333302</v>
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="C43">
+        <v>0.81</v>
       </c>
       <c r="D43">
         <v>0.85909090909090902</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>0.155555555555555</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.68333333333333302</v>
+        <v>0.7</v>
+      </c>
+      <c r="C44">
+        <v>0.83</v>
       </c>
       <c r="D44">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>0.211111111111111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.78333333333333299</v>
+        <v>0.88333333333333297</v>
+      </c>
+      <c r="C45">
+        <v>0.82999999999999896</v>
       </c>
       <c r="D45">
         <v>0.85909090909090902</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>0.266666666666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
         <v>0.76666666666666605</v>
       </c>
+      <c r="C46">
+        <v>0.76999999999999902</v>
+      </c>
       <c r="D46">
         <v>0.86363636363636298</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>0.16111111111111101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.91666666666666596</v>
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="C47">
+        <v>0.84</v>
       </c>
       <c r="D47">
         <v>0.76818181818181797</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>0.24444444444444399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.78333333333333299</v>
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="C48">
+        <v>0.80999999999999905</v>
       </c>
       <c r="D48">
         <v>0.85909090909090902</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>0.39444444444444399</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.76666666666666605</v>
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="C49">
+        <v>0.83</v>
       </c>
       <c r="D49">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>0.31111111111111101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.749999999999999</v>
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="C50">
+        <v>0.89</v>
       </c>
       <c r="D50">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>0.32222222222222202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.78333333333333299</v>
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="C51">
+        <v>0.91999999999999904</v>
       </c>
       <c r="D51">
         <v>0.88636363636363602</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>50</v>
-      </c>
-      <c r="D52">
-        <v>0.81363636363636305</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>51</v>
-      </c>
-      <c r="D53">
-        <v>0.88636363636363602</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="D54">
-        <v>0.90909090909090895</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>53</v>
-      </c>
-      <c r="D55">
-        <v>0.88636363636363602</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>54</v>
-      </c>
-      <c r="D56">
-        <v>0.88181818181818095</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>55</v>
-      </c>
-      <c r="D57">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>56</v>
-      </c>
-      <c r="D58">
-        <v>0.88636363636363602</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>57</v>
-      </c>
-      <c r="D59">
-        <v>0.79545454545454497</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>58</v>
-      </c>
-      <c r="D60">
-        <v>0.79545454545454497</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>59</v>
-      </c>
-      <c r="D61">
-        <v>0.83636363636363598</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>60</v>
-      </c>
-      <c r="D62">
-        <v>0.62727272727272698</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>61</v>
-      </c>
-      <c r="D63">
-        <v>0.81363636363636305</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>62</v>
-      </c>
-      <c r="D64">
-        <v>0.83636363636363598</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>63</v>
-      </c>
-      <c r="D65">
-        <v>0.84090909090909005</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>64</v>
-      </c>
-      <c r="D66">
-        <v>0.81363636363636305</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>65</v>
-      </c>
-      <c r="D67">
-        <v>0.72727272727272696</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>66</v>
-      </c>
-      <c r="D68">
-        <v>0.84090909090909005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>67</v>
-      </c>
-      <c r="D69">
-        <v>0.84090909090909005</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>68</v>
-      </c>
-      <c r="D70">
-        <v>0.78181818181818097</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>69</v>
-      </c>
-      <c r="D71">
-        <v>0.78181818181818197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>70</v>
-      </c>
-      <c r="D72">
-        <v>0.75909090909090904</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>71</v>
-      </c>
-      <c r="D73">
-        <v>0.736363636363636</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>72</v>
-      </c>
-      <c r="D74">
-        <v>0.81818181818181801</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>73</v>
-      </c>
-      <c r="D75">
-        <v>0.84090909090909005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>74</v>
-      </c>
-      <c r="D76">
-        <v>0.86363636363636298</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>75</v>
-      </c>
-      <c r="D77">
-        <v>0.90909090909090895</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>76</v>
-      </c>
-      <c r="D78">
-        <v>0.81818181818181801</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>77</v>
-      </c>
-      <c r="D79">
-        <v>0.777272727272727</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>78</v>
-      </c>
-      <c r="D80">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>79</v>
-      </c>
-      <c r="D81">
-        <v>0.75909090909090904</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>80</v>
-      </c>
-      <c r="D82">
-        <v>0.82727272727272705</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>81</v>
-      </c>
-      <c r="D83">
-        <v>0.81818181818181801</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>82</v>
-      </c>
-      <c r="D84">
-        <v>0.722727272727272</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>83</v>
-      </c>
-      <c r="D85">
-        <v>0.81818181818181801</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>84</v>
-      </c>
-      <c r="D86">
-        <v>0.69090909090909003</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>85</v>
-      </c>
-      <c r="D87">
-        <v>0.75909090909090904</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>86</v>
-      </c>
-      <c r="D88">
-        <v>0.83181818181818101</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>87</v>
-      </c>
-      <c r="D89">
-        <v>0.77272727272727204</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>88</v>
-      </c>
-      <c r="D90">
-        <v>0.84090909090909005</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>89</v>
-      </c>
-      <c r="D91">
-        <v>0.81363636363636305</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>90</v>
-      </c>
-      <c r="D92">
-        <v>0.72727272727272696</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>91</v>
-      </c>
-      <c r="D93">
-        <v>0.83636363636363598</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>92</v>
-      </c>
-      <c r="D94">
-        <v>0.77272727272727204</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>93</v>
-      </c>
-      <c r="D95">
-        <v>0.80909090909090897</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>94</v>
-      </c>
-      <c r="D96">
-        <v>0.75909090909090904</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>95</v>
-      </c>
-      <c r="D97">
-        <v>0.78636363636363604</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>96</v>
-      </c>
-      <c r="D98">
-        <v>0.83636363636363598</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>97</v>
-      </c>
-      <c r="D99">
-        <v>0.73181818181818103</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>98</v>
-      </c>
-      <c r="D100">
-        <v>0.79545454545454497</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>99</v>
-      </c>
-      <c r="D101">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="H51">
+        <v>0.27777777777777701</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="B102" t="s">
-        <v>8</v>
+      <c r="C52" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>